<commit_message>
Creating dynamic algorithms for position functions with regards to dynamic values of gravity and atmospheric density
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Interactive Resource Impact Simulation\Versions\IRIS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73042391-F10A-42F2-926A-4E235AFFC1B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,233 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i_max = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">j_max = </t>
+  </si>
+  <si>
+    <t>folder =</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>file =</t>
+  </si>
+  <si>
+    <t>Maximum number of j loops</t>
+  </si>
+  <si>
+    <t>Maximum number of i loops</t>
+  </si>
+  <si>
+    <t>d =</t>
+  </si>
+  <si>
+    <t>Diameter of pod (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m_p = </t>
+  </si>
+  <si>
+    <t>Mass of planet (kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m = </t>
+  </si>
+  <si>
+    <t>Mass of pod and contents (kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rho = </t>
+  </si>
+  <si>
+    <t>Atmospheric density (kg/m^3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y_p = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G_p = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">parachute = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">m_o = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_o = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_num = </t>
+  </si>
+  <si>
+    <t>Square root of faces of sphere</t>
+  </si>
+  <si>
+    <t>Area of parachute (m^2)</t>
+  </si>
+  <si>
+    <t>Mass of parachute (kg)</t>
+  </si>
+  <si>
+    <t>True/false for existence of parachute</t>
+  </si>
+  <si>
+    <t>Modulus of Rigidity of pod shell (gf/mm^2)</t>
+  </si>
+  <si>
+    <t>Young’s Modulus of pod shell (gf/mm^2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u_i = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_max = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_min = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_ max = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_min = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_r_max = </t>
+  </si>
+  <si>
+    <t>F_r_min =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K_max = </t>
+  </si>
+  <si>
+    <t>K_min =</t>
+  </si>
+  <si>
+    <t>T_c_max =</t>
+  </si>
+  <si>
+    <t>T_c_min =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G_l_max = </t>
+  </si>
+  <si>
+    <t>G_l_min =</t>
+  </si>
+  <si>
+    <t>T_g_max =</t>
+  </si>
+  <si>
+    <t>T_g_min =</t>
+  </si>
+  <si>
+    <t>Y_l_max =</t>
+  </si>
+  <si>
+    <t>Y_l_min =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">domain = </t>
+  </si>
+  <si>
+    <t>Horizontal width of considered terrain (m)</t>
+  </si>
+  <si>
+    <t>Maximum value of terrain surface (m)</t>
+  </si>
+  <si>
+    <t>Minimum value of terrain surface (m)</t>
+  </si>
+  <si>
+    <t>Maximum value of Coefficient of Friction between pod and surface</t>
+  </si>
+  <si>
+    <t>Minimum value of Coefficient of Friction between pod and surface</t>
+  </si>
+  <si>
+    <t>Maximum value of Coefficient of Rolling Friction between pod and surface</t>
+  </si>
+  <si>
+    <t>Minimum value of Coefficient of Rolling Friction between pod and surface</t>
+  </si>
+  <si>
+    <t>Maximum value of Coefficient of Restitution between pod and surface</t>
+  </si>
+  <si>
+    <t>Minimum value of Coefficient of Restitution between pod and surface</t>
+  </si>
+  <si>
+    <t>Maximum value of thermal conductivity between pod and surface (W/mK)</t>
+  </si>
+  <si>
+    <t>Minimum value of thermal conductivity between pod and surface (W/mK)</t>
+  </si>
+  <si>
+    <t>Maximum value of Modulus of Rigidity of surface (gf/mm^2)</t>
+  </si>
+  <si>
+    <t>Minimum value of Modulus of Rigidity of surface (gf/mm^2)</t>
+  </si>
+  <si>
+    <t>Maximum value of temperature of surface (K)</t>
+  </si>
+  <si>
+    <t>Minimum value of temperature of surface (K)</t>
+  </si>
+  <si>
+    <t>Maximum value of Young's Modulus of surface (gf/mm^2)</t>
+  </si>
+  <si>
+    <t>Minimum value of Young's Modulus of surface (gf/mm^2)</t>
+  </si>
+  <si>
+    <t>Vector defining initial velocity of pod (m/s) [u_i(1,3) being altitude above L_min]</t>
+  </si>
+  <si>
+    <t>5.972*10^24</t>
+  </si>
+  <si>
+    <t>[0,0,1000000;0,0,0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t_o = </t>
+  </si>
+  <si>
+    <t>Time of parachute opening on supply pod drop (s)</t>
+  </si>
+  <si>
+    <t>'Empty'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t_A_int = </t>
+  </si>
+  <si>
+    <t>Intervals of differences in atmospheric/gravity conditions for trajectory (s)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +258,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,14 +303,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{BDC23125-5662-449E-AB6C-355338C5F832}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +614,393 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35:D35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.1328125" customWidth="1"/>
+    <col min="2" max="2" width="65.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.9296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.06640625" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="2"/>
+      <c r="B4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="2"/>
+      <c r="B5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="2"/>
+      <c r="B6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="7">
+        <v>6371000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="2"/>
+      <c r="B7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="2"/>
+      <c r="B8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="2"/>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="2"/>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="2"/>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="2"/>
+      <c r="B20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="9">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B34" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C37" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Averaging point of gravity and atmosphere for x and y coordinates
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Interactive Resource Impact Simulation\Versions\IRIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73042391-F10A-42F2-926A-4E235AFFC1B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDDF744-FE98-42E3-9BE0-4575CFE5CD74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,9 +228,6 @@
     <t>5.972*10^24</t>
   </si>
   <si>
-    <t>[0,0,1000000;0,0,0]</t>
-  </si>
-  <si>
     <t xml:space="preserve">t_o = </t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>Intervals of differences in atmospheric/gravity conditions for trajectory (s)</t>
+  </si>
+  <si>
+    <t>[-50,0,1000000;-0,50,50]</t>
   </si>
 </sst>
 </file>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:D35"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -658,7 +658,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -952,10 +952,10 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32" s="9">
         <v>400</v>
@@ -979,18 +979,18 @@
         <v>30</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D35" s="9">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Improving collision search algorithm to be more efficient and modular
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Interactive Resource Impact Simulation\Versions\IRIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDDF744-FE98-42E3-9BE0-4575CFE5CD74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2203AA7A-DEE2-46C6-A7EB-D002981B9B2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Variables</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>[-50,0,1000000;-0,50,50]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t_step = </t>
+  </si>
+  <si>
+    <t>Intervals of steps of pod search along trajectory (s)</t>
   </si>
 </sst>
 </file>
@@ -617,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -993,6 +999,14 @@
         <v>10000</v>
       </c>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C37" s="10"/>
     </row>

</xml_diff>

<commit_message>
Fixing issues in segment\final.m
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Interactive Resource Impact Simulation\Versions\IRIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66763AAD-F5A1-4050-9CBF-F052A779D08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F202905-60DF-4AC6-A482-A7940694BCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Variables</t>
   </si>
@@ -274,6 +274,24 @@
   </si>
   <si>
     <t>Initial temperature of pod (K)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_H = </t>
+  </si>
+  <si>
+    <t>Stiffness of pod shell (N/m^1.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T = </t>
+  </si>
+  <si>
+    <t>Length of time segments (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B_m_min = </t>
+  </si>
+  <si>
+    <t>Minimum value of perpendicular vector (m/s)</t>
   </si>
 </sst>
 </file>
@@ -644,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1075,6 +1093,30 @@
         <v>81</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B42" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B43" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:D1"/>

</xml_diff>

<commit_message>
Input variables test completion
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Interactive Resource Impact Simulation\Versions\IRIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3F6397-E003-43EA-AABC-4DE54CA32D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00BCC45-169D-4422-AC38-5811422EF7B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -773,7 +773,7 @@
   <dimension ref="B1:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>